<commit_message>
fix: Updated Excel import data - all 215 dates now valid
</commit_message>
<xml_diff>
--- a/Poker results.xlsx
+++ b/Poker results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\פרטי\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liormol\projects\Poker Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0FC5086-178F-4261-A603-72D3B6D4EF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D3767E-7C21-4370-9B42-F9694FFA7F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{531639C6-E4BF-45C3-88E8-5B5EA68868B7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>תומר</t>
   </si>
@@ -188,9 +188,6 @@
     <t>22/06/24</t>
   </si>
   <si>
-    <t>ינואר22</t>
-  </si>
-  <si>
     <t>25/12/21</t>
   </si>
   <si>
@@ -213,9 +210,6 @@
   </si>
   <si>
     <t>21/08/21</t>
-  </si>
-  <si>
-    <t>07/108/21</t>
   </si>
   <si>
     <t>17/07/21</t>
@@ -254,20 +248,20 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -276,7 +270,7 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -377,6 +371,11 @@
   <dxfs count="100">
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF00B050"/>
       </font>
     </dxf>
@@ -414,6 +413,21 @@
       <font>
         <color rgb="FF9C0006"/>
       </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -432,6 +446,226 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -637,6 +871,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -652,6 +896,116 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -777,21 +1131,21 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -877,16 +1231,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -902,356 +1246,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1627,84 +1621,84 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70A305C-45BC-4413-B0CD-355998277BD6}">
   <dimension ref="B11:HK51"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="F9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="11" spans="2:219" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B11" s="22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H11" s="21">
         <v>44322</v>
       </c>
       <c r="I11" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="J11" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="J11" s="21">
+        <v>44415</v>
       </c>
       <c r="K11" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L11" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M11" s="21">
         <v>44206</v>
       </c>
       <c r="N11" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O11" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P11" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q11" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R11" s="21">
         <v>44298</v>
       </c>
       <c r="S11" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="T11" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="U11" s="21" t="s">
         <v>50</v>
       </c>
+      <c r="U11" s="21">
+        <v>44562</v>
+      </c>
       <c r="V11" s="21">
-        <v>5.0199999999999996</v>
+        <v>44566.02</v>
       </c>
       <c r="W11" s="21">
-        <v>12.02</v>
+        <v>44573.02</v>
       </c>
       <c r="X11" s="21">
-        <v>26.02</v>
+        <v>44587.02</v>
       </c>
       <c r="Y11" s="21">
-        <v>5.03</v>
+        <v>44566.03</v>
       </c>
       <c r="Z11" s="21">
         <v>44639</v>
@@ -2289,7 +2283,7 @@
         <v>46004</v>
       </c>
     </row>
-    <row r="12" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>39</v>
       </c>
@@ -2845,7 +2839,7 @@
         <v>306.14999999999998</v>
       </c>
     </row>
-    <row r="13" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>38</v>
       </c>
@@ -3357,7 +3351,7 @@
         <v>251.39999999999998</v>
       </c>
     </row>
-    <row r="14" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>37</v>
       </c>
@@ -3755,7 +3749,7 @@
       <c r="HJ14" s="1"/>
       <c r="HK14" s="1"/>
     </row>
-    <row r="15" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>36</v>
       </c>
@@ -4025,7 +4019,7 @@
       <c r="HJ15" s="1"/>
       <c r="HK15" s="1"/>
     </row>
-    <row r="16" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>35</v>
       </c>
@@ -4253,7 +4247,7 @@
       <c r="HJ16" s="1"/>
       <c r="HK16" s="1"/>
     </row>
-    <row r="17" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>34</v>
       </c>
@@ -4885,7 +4879,7 @@
         <v>-120</v>
       </c>
     </row>
-    <row r="18" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>33</v>
       </c>
@@ -5173,7 +5167,7 @@
       <c r="HJ18" s="1"/>
       <c r="HK18" s="1"/>
     </row>
-    <row r="19" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>32</v>
       </c>
@@ -5397,7 +5391,7 @@
       <c r="HJ19" s="1"/>
       <c r="HK19" s="1"/>
     </row>
-    <row r="20" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>31</v>
       </c>
@@ -5917,7 +5911,7 @@
         <v>-120</v>
       </c>
     </row>
-    <row r="21" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
         <v>30</v>
       </c>
@@ -6151,7 +6145,7 @@
       </c>
       <c r="HK21" s="1"/>
     </row>
-    <row r="22" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
         <v>29</v>
       </c>
@@ -6379,7 +6373,7 @@
       <c r="HJ22" s="1"/>
       <c r="HK22" s="1"/>
     </row>
-    <row r="23" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
         <v>28</v>
       </c>
@@ -6603,7 +6597,7 @@
       <c r="HJ23" s="1"/>
       <c r="HK23" s="1"/>
     </row>
-    <row r="24" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
         <v>27</v>
       </c>
@@ -6831,7 +6825,7 @@
       <c r="HJ24" s="1"/>
       <c r="HK24" s="1"/>
     </row>
-    <row r="25" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
         <v>26</v>
       </c>
@@ -7065,7 +7059,7 @@
       <c r="HJ25" s="1"/>
       <c r="HK25" s="1"/>
     </row>
-    <row r="26" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
         <v>25</v>
       </c>
@@ -7291,7 +7285,7 @@
       <c r="HJ26" s="1"/>
       <c r="HK26" s="1"/>
     </row>
-    <row r="27" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
         <v>24</v>
       </c>
@@ -7517,7 +7511,7 @@
       <c r="HJ27" s="1"/>
       <c r="HK27" s="1"/>
     </row>
-    <row r="28" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
         <v>23</v>
       </c>
@@ -7741,7 +7735,7 @@
       <c r="HJ28" s="1"/>
       <c r="HK28" s="1"/>
     </row>
-    <row r="29" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">
         <v>22</v>
       </c>
@@ -7965,7 +7959,7 @@
       <c r="HJ29" s="1"/>
       <c r="HK29" s="1"/>
     </row>
-    <row r="30" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="s">
         <v>21</v>
       </c>
@@ -8189,7 +8183,7 @@
       <c r="HJ30" s="1"/>
       <c r="HK30" s="1"/>
     </row>
-    <row r="31" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B31" s="7" t="s">
         <v>20</v>
       </c>
@@ -8541,7 +8535,7 @@
       <c r="HJ31" s="1"/>
       <c r="HK31" s="1"/>
     </row>
-    <row r="32" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B32" s="7" t="s">
         <v>19</v>
       </c>
@@ -8803,7 +8797,7 @@
       <c r="HJ32" s="1"/>
       <c r="HK32" s="1"/>
     </row>
-    <row r="33" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B33" s="7" t="s">
         <v>18</v>
       </c>
@@ -9031,7 +9025,7 @@
       <c r="HJ33" s="1"/>
       <c r="HK33" s="1"/>
     </row>
-    <row r="34" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B34" s="7" t="s">
         <v>17</v>
       </c>
@@ -9255,7 +9249,7 @@
       <c r="HJ34" s="1"/>
       <c r="HK34" s="1"/>
     </row>
-    <row r="35" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B35" s="7" t="s">
         <v>16</v>
       </c>
@@ -9479,7 +9473,7 @@
       <c r="HJ35" s="1"/>
       <c r="HK35" s="1"/>
     </row>
-    <row r="36" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B36" s="7" t="s">
         <v>15</v>
       </c>
@@ -9703,7 +9697,7 @@
       <c r="HJ36" s="1"/>
       <c r="HK36" s="1"/>
     </row>
-    <row r="37" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B37" s="7" t="s">
         <v>14</v>
       </c>
@@ -9935,7 +9929,7 @@
       <c r="HJ37" s="1"/>
       <c r="HK37" s="1"/>
     </row>
-    <row r="38" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B38" s="7" t="s">
         <v>13</v>
       </c>
@@ -10159,7 +10153,7 @@
       <c r="HJ38" s="1"/>
       <c r="HK38" s="1"/>
     </row>
-    <row r="39" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B39" s="7" t="s">
         <v>12</v>
       </c>
@@ -10401,7 +10395,7 @@
       <c r="HJ39" s="1"/>
       <c r="HK39" s="1"/>
     </row>
-    <row r="40" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B40" s="7" t="s">
         <v>11</v>
       </c>
@@ -10635,7 +10629,7 @@
       <c r="HJ40" s="1"/>
       <c r="HK40" s="1"/>
     </row>
-    <row r="41" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B41" s="7" t="s">
         <v>10</v>
       </c>
@@ -10887,7 +10881,7 @@
       <c r="HJ41" s="1"/>
       <c r="HK41" s="1"/>
     </row>
-    <row r="42" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B42" s="7" t="s">
         <v>9</v>
       </c>
@@ -11121,7 +11115,7 @@
       <c r="HJ42" s="1"/>
       <c r="HK42" s="1"/>
     </row>
-    <row r="43" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B43" s="7" t="s">
         <v>8</v>
       </c>
@@ -11345,7 +11339,7 @@
       <c r="HJ43" s="1"/>
       <c r="HK43" s="1"/>
     </row>
-    <row r="44" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B44" s="7" t="s">
         <v>7</v>
       </c>
@@ -11569,7 +11563,7 @@
       <c r="HJ44" s="1"/>
       <c r="HK44" s="1"/>
     </row>
-    <row r="45" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B45" s="7" t="s">
         <v>6</v>
       </c>
@@ -11857,7 +11851,7 @@
       <c r="HJ45" s="1"/>
       <c r="HK45" s="1"/>
     </row>
-    <row r="46" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B46" s="7" t="s">
         <v>5</v>
       </c>
@@ -12271,7 +12265,7 @@
         <v>-90</v>
       </c>
     </row>
-    <row r="47" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B47" s="7" t="s">
         <v>4</v>
       </c>
@@ -12705,7 +12699,7 @@
       <c r="HJ47" s="1"/>
       <c r="HK47" s="1"/>
     </row>
-    <row r="48" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B48" s="7" t="s">
         <v>3</v>
       </c>
@@ -13113,7 +13107,7 @@
         <v>-275.85000000000002</v>
       </c>
     </row>
-    <row r="49" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B49" s="7" t="s">
         <v>2</v>
       </c>
@@ -13371,7 +13365,7 @@
       <c r="HJ49" s="1"/>
       <c r="HK49" s="1"/>
     </row>
-    <row r="50" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B50" s="7" t="s">
         <v>1</v>
       </c>
@@ -13815,7 +13809,7 @@
         <v>78.3</v>
       </c>
     </row>
-    <row r="51" spans="2:219" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:219" x14ac:dyDescent="0.25">
       <c r="B51" s="7" t="s">
         <v>0</v>
       </c>
@@ -14299,8 +14293,8 @@
     <cfRule type="top10" dxfId="92" priority="24" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:F51">
-    <cfRule type="top10" dxfId="91" priority="25" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="90" priority="26" rank="1"/>
+    <cfRule type="top10" dxfId="91" priority="26" rank="1"/>
+    <cfRule type="top10" dxfId="90" priority="25" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:G51">
     <cfRule type="top10" dxfId="89" priority="27" bottom="1" rank="1"/>
@@ -14319,8 +14313,8 @@
     <cfRule type="top10" dxfId="82" priority="34" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12:K51">
-    <cfRule type="top10" dxfId="81" priority="35" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="80" priority="36" rank="1"/>
+    <cfRule type="top10" dxfId="81" priority="36" rank="1"/>
+    <cfRule type="top10" dxfId="80" priority="35" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L12:L51">
     <cfRule type="top10" dxfId="79" priority="37" bottom="1" rank="1"/>
@@ -14347,32 +14341,32 @@
     <cfRule type="top10" dxfId="68" priority="48" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R12:R51">
-    <cfRule type="top10" dxfId="67" priority="49" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="66" priority="50" rank="1"/>
+    <cfRule type="top10" dxfId="67" priority="50" rank="1"/>
+    <cfRule type="top10" dxfId="66" priority="49" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S12:S51">
     <cfRule type="top10" dxfId="65" priority="51" bottom="1" rank="1"/>
     <cfRule type="top10" dxfId="64" priority="52" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T12:T51">
-    <cfRule type="top10" dxfId="63" priority="53" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="62" priority="54" rank="1"/>
+    <cfRule type="top10" dxfId="63" priority="54" rank="1"/>
+    <cfRule type="top10" dxfId="62" priority="53" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U12:U51">
     <cfRule type="top10" dxfId="61" priority="55" bottom="1" rank="1"/>
     <cfRule type="top10" dxfId="60" priority="56" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="V12:V51">
-    <cfRule type="top10" dxfId="59" priority="57" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="58" priority="58" rank="1"/>
+    <cfRule type="top10" dxfId="59" priority="58" rank="1"/>
+    <cfRule type="top10" dxfId="58" priority="57" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="W12:W51">
-    <cfRule type="top10" dxfId="57" priority="59" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="56" priority="60" rank="1"/>
+    <cfRule type="top10" dxfId="57" priority="60" rank="1"/>
+    <cfRule type="top10" dxfId="56" priority="59" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="X12:X51">
-    <cfRule type="top10" dxfId="55" priority="61" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="54" priority="62" rank="1"/>
+    <cfRule type="top10" dxfId="55" priority="62" rank="1"/>
+    <cfRule type="top10" dxfId="54" priority="61" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y12:Y51">
     <cfRule type="top10" dxfId="53" priority="63" bottom="1" rank="1"/>
@@ -14415,8 +14409,8 @@
     <cfRule type="top10" dxfId="34" priority="82" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI12:AI51">
-    <cfRule type="top10" dxfId="33" priority="17" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="32" priority="18" rank="1"/>
+    <cfRule type="top10" dxfId="33" priority="18" rank="1"/>
+    <cfRule type="top10" dxfId="32" priority="17" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ12:AJ51">
     <cfRule type="top10" dxfId="31" priority="83" bottom="1" rank="1"/>
@@ -14427,16 +14421,16 @@
     <cfRule type="top10" dxfId="28" priority="86" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL12:AL51 AO12:AO51">
-    <cfRule type="top10" dxfId="27" priority="87" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="26" priority="88" rank="1"/>
+    <cfRule type="top10" dxfId="27" priority="88" rank="1"/>
+    <cfRule type="top10" dxfId="26" priority="87" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM12:AM51">
-    <cfRule type="top10" dxfId="25" priority="15" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="24" priority="16" rank="1"/>
+    <cfRule type="top10" dxfId="25" priority="16" rank="1"/>
+    <cfRule type="top10" dxfId="24" priority="15" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN12:AN51">
-    <cfRule type="top10" dxfId="23" priority="13" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="22" priority="14" rank="1"/>
+    <cfRule type="top10" dxfId="23" priority="14" rank="1"/>
+    <cfRule type="top10" dxfId="22" priority="13" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP12:AP51">
     <cfRule type="top10" dxfId="21" priority="89" bottom="1" rank="1"/>
@@ -14463,38 +14457,38 @@
     <cfRule type="top10" dxfId="10" priority="100" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV12:AV51">
-    <cfRule type="top10" dxfId="9" priority="7" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="8" priority="8" rank="1"/>
+    <cfRule type="top10" dxfId="9" priority="8" rank="1"/>
+    <cfRule type="top10" dxfId="8" priority="7" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV13:CD15">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV16:CD51">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV12:EW12">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA14:HK51 C19:AV20">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix: Update Excel with corrected dates, ignore temp files
</commit_message>
<xml_diff>
--- a/Poker results.xlsx
+++ b/Poker results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liormol\projects\Poker Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D3767E-7C21-4370-9B42-F9694FFA7F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3937F44D-2EF2-485E-81D8-B9CA6B997E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{531639C6-E4BF-45C3-88E8-5B5EA68868B7}"/>
   </bookViews>
@@ -1622,7 +1622,7 @@
   <dimension ref="B11:HK51"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" topLeftCell="F9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1698,7 +1698,7 @@
         <v>44587.02</v>
       </c>
       <c r="Y11" s="21">
-        <v>44566.03</v>
+        <v>44591.03</v>
       </c>
       <c r="Z11" s="21">
         <v>44639</v>

</xml_diff>

<commit_message>
v3.6.1: Import reads player types from Excel column A
</commit_message>
<xml_diff>
--- a/Poker results.xlsx
+++ b/Poker results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liormol\projects\Poker Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394D79C0-75F3-4C1E-B796-333163AA4968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A8F9C3-F169-42A1-92BF-F8390CABD966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{531639C6-E4BF-45C3-88E8-5B5EA68868B7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="68">
   <si>
     <t>תומר</t>
   </si>
@@ -231,6 +231,15 @@
   </si>
   <si>
     <t>שחקן</t>
+  </si>
+  <si>
+    <t>קבוע</t>
+  </si>
+  <si>
+    <t>אורח</t>
+  </si>
+  <si>
+    <t>מזדמן</t>
   </si>
 </sst>
 </file>
@@ -1619,15 +1628,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70A305C-45BC-4413-B0CD-355998277BD6}">
-  <dimension ref="B11:HK51"/>
+  <dimension ref="A11:HK51"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="F9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y12" sqref="Y12"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="11" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:219" x14ac:dyDescent="0.25">
       <c r="B11" s="22" t="s">
         <v>64</v>
       </c>
@@ -2283,7 +2292,10 @@
         <v>46004</v>
       </c>
     </row>
-    <row r="12" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
       <c r="B12" s="7" t="s">
         <v>39</v>
       </c>
@@ -2836,10 +2848,13 @@
         <v>141.5</v>
       </c>
       <c r="HK12" s="1">
-        <v>306.14999999999998</v>
+        <v>321.14999999999998</v>
       </c>
     </row>
-    <row r="13" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>65</v>
+      </c>
       <c r="B13" s="7" t="s">
         <v>38</v>
       </c>
@@ -3348,10 +3363,13 @@
         <v>119.3</v>
       </c>
       <c r="HK13" s="1">
-        <v>251.39999999999998</v>
+        <v>266.39999999999998</v>
       </c>
     </row>
-    <row r="14" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
       <c r="B14" s="7" t="s">
         <v>37</v>
       </c>
@@ -3749,7 +3767,10 @@
       <c r="HJ14" s="1"/>
       <c r="HK14" s="1"/>
     </row>
-    <row r="15" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
       <c r="B15" s="7" t="s">
         <v>36</v>
       </c>
@@ -4019,7 +4040,10 @@
       <c r="HJ15" s="1"/>
       <c r="HK15" s="1"/>
     </row>
-    <row r="16" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>67</v>
+      </c>
       <c r="B16" s="7" t="s">
         <v>35</v>
       </c>
@@ -4247,7 +4271,10 @@
       <c r="HJ16" s="1"/>
       <c r="HK16" s="1"/>
     </row>
-    <row r="17" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>65</v>
+      </c>
       <c r="B17" s="8" t="s">
         <v>34</v>
       </c>
@@ -4876,10 +4903,13 @@
         <v>98.4</v>
       </c>
       <c r="HK17" s="9">
-        <v>-120</v>
+        <v>-150</v>
       </c>
     </row>
-    <row r="18" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>66</v>
+      </c>
       <c r="B18" s="7" t="s">
         <v>33</v>
       </c>
@@ -5167,7 +5197,10 @@
       <c r="HJ18" s="1"/>
       <c r="HK18" s="1"/>
     </row>
-    <row r="19" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
       <c r="B19" s="7" t="s">
         <v>32</v>
       </c>
@@ -5391,7 +5424,10 @@
       <c r="HJ19" s="1"/>
       <c r="HK19" s="1"/>
     </row>
-    <row r="20" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>65</v>
+      </c>
       <c r="B20" s="7" t="s">
         <v>31</v>
       </c>
@@ -5911,7 +5947,10 @@
         <v>-120</v>
       </c>
     </row>
-    <row r="21" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>65</v>
+      </c>
       <c r="B21" s="8" t="s">
         <v>30</v>
       </c>
@@ -6145,7 +6184,10 @@
       </c>
       <c r="HK21" s="1"/>
     </row>
-    <row r="22" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>67</v>
+      </c>
       <c r="B22" s="7" t="s">
         <v>29</v>
       </c>
@@ -6373,7 +6415,10 @@
       <c r="HJ22" s="1"/>
       <c r="HK22" s="1"/>
     </row>
-    <row r="23" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
       <c r="B23" s="7" t="s">
         <v>28</v>
       </c>
@@ -6597,7 +6642,10 @@
       <c r="HJ23" s="1"/>
       <c r="HK23" s="1"/>
     </row>
-    <row r="24" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>67</v>
+      </c>
       <c r="B24" s="7" t="s">
         <v>27</v>
       </c>
@@ -6825,7 +6873,10 @@
       <c r="HJ24" s="1"/>
       <c r="HK24" s="1"/>
     </row>
-    <row r="25" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>67</v>
+      </c>
       <c r="B25" s="7" t="s">
         <v>26</v>
       </c>
@@ -7059,7 +7110,10 @@
       <c r="HJ25" s="1"/>
       <c r="HK25" s="1"/>
     </row>
-    <row r="26" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>67</v>
+      </c>
       <c r="B26" s="7" t="s">
         <v>25</v>
       </c>
@@ -7285,7 +7339,10 @@
       <c r="HJ26" s="1"/>
       <c r="HK26" s="1"/>
     </row>
-    <row r="27" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>67</v>
+      </c>
       <c r="B27" s="7" t="s">
         <v>24</v>
       </c>
@@ -7511,7 +7568,10 @@
       <c r="HJ27" s="1"/>
       <c r="HK27" s="1"/>
     </row>
-    <row r="28" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>67</v>
+      </c>
       <c r="B28" s="7" t="s">
         <v>23</v>
       </c>
@@ -7735,7 +7795,10 @@
       <c r="HJ28" s="1"/>
       <c r="HK28" s="1"/>
     </row>
-    <row r="29" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
       <c r="B29" s="7" t="s">
         <v>22</v>
       </c>
@@ -7959,7 +8022,10 @@
       <c r="HJ29" s="1"/>
       <c r="HK29" s="1"/>
     </row>
-    <row r="30" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>67</v>
+      </c>
       <c r="B30" s="7" t="s">
         <v>21</v>
       </c>
@@ -8183,7 +8249,10 @@
       <c r="HJ30" s="1"/>
       <c r="HK30" s="1"/>
     </row>
-    <row r="31" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>67</v>
+      </c>
       <c r="B31" s="7" t="s">
         <v>20</v>
       </c>
@@ -8535,7 +8604,10 @@
       <c r="HJ31" s="1"/>
       <c r="HK31" s="1"/>
     </row>
-    <row r="32" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>67</v>
+      </c>
       <c r="B32" s="7" t="s">
         <v>19</v>
       </c>
@@ -8797,7 +8869,10 @@
       <c r="HJ32" s="1"/>
       <c r="HK32" s="1"/>
     </row>
-    <row r="33" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>67</v>
+      </c>
       <c r="B33" s="7" t="s">
         <v>18</v>
       </c>
@@ -9025,7 +9100,10 @@
       <c r="HJ33" s="1"/>
       <c r="HK33" s="1"/>
     </row>
-    <row r="34" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>67</v>
+      </c>
       <c r="B34" s="7" t="s">
         <v>17</v>
       </c>
@@ -9249,7 +9327,10 @@
       <c r="HJ34" s="1"/>
       <c r="HK34" s="1"/>
     </row>
-    <row r="35" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>67</v>
+      </c>
       <c r="B35" s="7" t="s">
         <v>16</v>
       </c>
@@ -9473,7 +9554,10 @@
       <c r="HJ35" s="1"/>
       <c r="HK35" s="1"/>
     </row>
-    <row r="36" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>67</v>
+      </c>
       <c r="B36" s="7" t="s">
         <v>15</v>
       </c>
@@ -9697,7 +9781,10 @@
       <c r="HJ36" s="1"/>
       <c r="HK36" s="1"/>
     </row>
-    <row r="37" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>67</v>
+      </c>
       <c r="B37" s="7" t="s">
         <v>14</v>
       </c>
@@ -9929,7 +10016,10 @@
       <c r="HJ37" s="1"/>
       <c r="HK37" s="1"/>
     </row>
-    <row r="38" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>67</v>
+      </c>
       <c r="B38" s="7" t="s">
         <v>13</v>
       </c>
@@ -10153,7 +10243,10 @@
       <c r="HJ38" s="1"/>
       <c r="HK38" s="1"/>
     </row>
-    <row r="39" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>67</v>
+      </c>
       <c r="B39" s="7" t="s">
         <v>12</v>
       </c>
@@ -10395,7 +10488,10 @@
       <c r="HJ39" s="1"/>
       <c r="HK39" s="1"/>
     </row>
-    <row r="40" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>67</v>
+      </c>
       <c r="B40" s="7" t="s">
         <v>11</v>
       </c>
@@ -10629,7 +10725,10 @@
       <c r="HJ40" s="1"/>
       <c r="HK40" s="1"/>
     </row>
-    <row r="41" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>66</v>
+      </c>
       <c r="B41" s="7" t="s">
         <v>10</v>
       </c>
@@ -10881,7 +10980,10 @@
       <c r="HJ41" s="1"/>
       <c r="HK41" s="1"/>
     </row>
-    <row r="42" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>67</v>
+      </c>
       <c r="B42" s="7" t="s">
         <v>9</v>
       </c>
@@ -11115,7 +11217,10 @@
       <c r="HJ42" s="1"/>
       <c r="HK42" s="1"/>
     </row>
-    <row r="43" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>67</v>
+      </c>
       <c r="B43" s="7" t="s">
         <v>8</v>
       </c>
@@ -11339,7 +11444,10 @@
       <c r="HJ43" s="1"/>
       <c r="HK43" s="1"/>
     </row>
-    <row r="44" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>67</v>
+      </c>
       <c r="B44" s="7" t="s">
         <v>7</v>
       </c>
@@ -11563,7 +11671,10 @@
       <c r="HJ44" s="1"/>
       <c r="HK44" s="1"/>
     </row>
-    <row r="45" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>66</v>
+      </c>
       <c r="B45" s="7" t="s">
         <v>6</v>
       </c>
@@ -11851,7 +11962,10 @@
       <c r="HJ45" s="1"/>
       <c r="HK45" s="1"/>
     </row>
-    <row r="46" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>65</v>
+      </c>
       <c r="B46" s="7" t="s">
         <v>5</v>
       </c>
@@ -12265,7 +12379,10 @@
         <v>-90</v>
       </c>
     </row>
-    <row r="47" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>65</v>
+      </c>
       <c r="B47" s="7" t="s">
         <v>4</v>
       </c>
@@ -12699,7 +12816,10 @@
       <c r="HJ47" s="1"/>
       <c r="HK47" s="1"/>
     </row>
-    <row r="48" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>65</v>
+      </c>
       <c r="B48" s="7" t="s">
         <v>3</v>
       </c>
@@ -13107,7 +13227,10 @@
         <v>-275.85000000000002</v>
       </c>
     </row>
-    <row r="49" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>66</v>
+      </c>
       <c r="B49" s="7" t="s">
         <v>2</v>
       </c>
@@ -13365,7 +13488,10 @@
       <c r="HJ49" s="1"/>
       <c r="HK49" s="1"/>
     </row>
-    <row r="50" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>65</v>
+      </c>
       <c r="B50" s="7" t="s">
         <v>1</v>
       </c>
@@ -13809,7 +13935,10 @@
         <v>78.3</v>
       </c>
     </row>
-    <row r="51" spans="2:219" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>65</v>
+      </c>
       <c r="B51" s="7" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
v4.6.1: Simplified active players filter - 33% of total games
</commit_message>
<xml_diff>
--- a/Poker results.xlsx
+++ b/Poker results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liormol\projects\Poker Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A8F9C3-F169-42A1-92BF-F8390CABD966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B010656-1E40-4424-903A-EB891C5279D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{531639C6-E4BF-45C3-88E8-5B5EA68868B7}"/>
   </bookViews>
@@ -1630,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70A305C-45BC-4413-B0CD-355998277BD6}">
   <dimension ref="A11:HK51"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4903,7 +4903,7 @@
         <v>98.4</v>
       </c>
       <c r="HK17" s="9">
-        <v>-150</v>
+        <v>-120</v>
       </c>
     </row>
     <row r="18" spans="1:219" x14ac:dyDescent="0.25">
@@ -5944,7 +5944,7 @@
         <v>-240</v>
       </c>
       <c r="HK20" s="1">
-        <v>-120</v>
+        <v>-150</v>
       </c>
     </row>
     <row r="21" spans="1:219" x14ac:dyDescent="0.25">
@@ -13193,7 +13193,7 @@
       </c>
       <c r="GS48" s="1"/>
       <c r="GT48" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="GU48" s="1"/>
       <c r="GV48" s="1"/>

</xml_diff>

<commit_message>
v4.6.3: Fix - Renamed All-Time Leaders to Hebrew, records reflect selected period
</commit_message>
<xml_diff>
--- a/Poker results.xlsx
+++ b/Poker results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liormol\projects\Poker Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B010656-1E40-4424-903A-EB891C5279D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76ED3498-E6F4-4329-93E2-B824393B0F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{531639C6-E4BF-45C3-88E8-5B5EA68868B7}"/>
   </bookViews>
@@ -1630,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70A305C-45BC-4413-B0CD-355998277BD6}">
   <dimension ref="A11:HK51"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K54" sqref="K54"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="HA1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="HQ20" sqref="HQ20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5778,7 +5778,7 @@
         <v>116.9</v>
       </c>
       <c r="EW20" s="3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="EX20" s="2"/>
       <c r="EY20" s="2">
@@ -5868,7 +5868,7 @@
         <v>0.01</v>
       </c>
       <c r="GG20" s="1">
-        <v>0</v>
+        <v>-65.900000000000006</v>
       </c>
       <c r="GH20" s="1">
         <v>-65.900000000000006</v>
@@ -5884,7 +5884,7 @@
         <v>-120</v>
       </c>
       <c r="GO20" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="GP20" s="1">
         <v>296</v>
@@ -5896,7 +5896,7 @@
         <v>-60</v>
       </c>
       <c r="GS20" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="GT20" s="1">
         <v>11.1</v>
@@ -11193,7 +11193,7 @@
       <c r="GR42" s="1"/>
       <c r="GS42" s="1"/>
       <c r="GT42" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="GU42" s="1"/>
       <c r="GV42" s="1"/>
@@ -13594,7 +13594,7 @@
         <v>424</v>
       </c>
       <c r="AQ50" s="3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AR50" s="3"/>
       <c r="AS50" s="3"/>
@@ -14613,7 +14613,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CA14:HK51 C19:AV20">
+  <conditionalFormatting sqref="C19:AV20 CA14:HK51">
     <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Add prepared date to import file, update import data
</commit_message>
<xml_diff>
--- a/Poker results.xlsx
+++ b/Poker results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liormol\projects\Poker Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76ED3498-E6F4-4329-93E2-B824393B0F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BE88FA-2F92-41B0-A21C-27270920DD8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{531639C6-E4BF-45C3-88E8-5B5EA68868B7}"/>
   </bookViews>
@@ -1630,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70A305C-45BC-4413-B0CD-355998277BD6}">
   <dimension ref="A11:HK51"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="HA1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="HQ20" sqref="HQ20"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="GU1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="HH24" sqref="HH24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
v4.9.9: AI Forecast enhanced creativity - random seed, varied styles, never boring
</commit_message>
<xml_diff>
--- a/Poker results.xlsx
+++ b/Poker results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liormol\projects\Poker Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BE88FA-2F92-41B0-A21C-27270920DD8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B20AF2D-76C8-43EC-8C90-89C2B734A0B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{531639C6-E4BF-45C3-88E8-5B5EA68868B7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="69">
   <si>
     <t>תומר</t>
   </si>
@@ -233,13 +233,16 @@
     <t>שחקן</t>
   </si>
   <si>
-    <t>קבוע</t>
+    <t>סוג שחקן</t>
   </si>
   <si>
-    <t>אורח</t>
+    <t>permanent</t>
   </si>
   <si>
-    <t>מזדמן</t>
+    <t>permanent guest</t>
+  </si>
+  <si>
+    <t>occasional</t>
   </si>
 </sst>
 </file>
@@ -1630,13 +1633,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70A305C-45BC-4413-B0CD-355998277BD6}">
   <dimension ref="A11:HK51"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="GU1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="HH24" sqref="HH24"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="11" spans="1:219" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
       <c r="B11" s="22" t="s">
         <v>64</v>
       </c>
@@ -2294,7 +2300,7 @@
     </row>
     <row r="12" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>39</v>
@@ -2853,7 +2859,7 @@
     </row>
     <row r="13" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>38</v>
@@ -3368,7 +3374,7 @@
     </row>
     <row r="14" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>37</v>
@@ -3769,7 +3775,7 @@
     </row>
     <row r="15" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>36</v>
@@ -4042,7 +4048,7 @@
     </row>
     <row r="16" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>35</v>
@@ -4273,7 +4279,7 @@
     </row>
     <row r="17" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>34</v>
@@ -4908,7 +4914,7 @@
     </row>
     <row r="18" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>33</v>
@@ -5199,7 +5205,7 @@
     </row>
     <row r="19" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>32</v>
@@ -5426,7 +5432,7 @@
     </row>
     <row r="20" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>31</v>
@@ -5949,7 +5955,7 @@
     </row>
     <row r="21" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>30</v>
@@ -6186,7 +6192,7 @@
     </row>
     <row r="22" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>29</v>
@@ -6417,7 +6423,7 @@
     </row>
     <row r="23" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>28</v>
@@ -6644,7 +6650,7 @@
     </row>
     <row r="24" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>27</v>
@@ -6875,7 +6881,7 @@
     </row>
     <row r="25" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>26</v>
@@ -7112,7 +7118,7 @@
     </row>
     <row r="26" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>25</v>
@@ -7341,7 +7347,7 @@
     </row>
     <row r="27" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>24</v>
@@ -7570,7 +7576,7 @@
     </row>
     <row r="28" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>23</v>
@@ -7797,7 +7803,7 @@
     </row>
     <row r="29" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>22</v>
@@ -8024,7 +8030,7 @@
     </row>
     <row r="30" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>21</v>
@@ -8251,7 +8257,7 @@
     </row>
     <row r="31" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>20</v>
@@ -8606,7 +8612,7 @@
     </row>
     <row r="32" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>19</v>
@@ -8871,7 +8877,7 @@
     </row>
     <row r="33" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>18</v>
@@ -9102,7 +9108,7 @@
     </row>
     <row r="34" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>17</v>
@@ -9329,7 +9335,7 @@
     </row>
     <row r="35" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>16</v>
@@ -9556,7 +9562,7 @@
     </row>
     <row r="36" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>15</v>
@@ -9783,7 +9789,7 @@
     </row>
     <row r="37" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>14</v>
@@ -10018,7 +10024,7 @@
     </row>
     <row r="38" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>13</v>
@@ -10245,7 +10251,7 @@
     </row>
     <row r="39" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>12</v>
@@ -10490,7 +10496,7 @@
     </row>
     <row r="40" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>11</v>
@@ -10727,7 +10733,7 @@
     </row>
     <row r="41" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>10</v>
@@ -10982,7 +10988,7 @@
     </row>
     <row r="42" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>9</v>
@@ -11219,7 +11225,7 @@
     </row>
     <row r="43" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>8</v>
@@ -11446,7 +11452,7 @@
     </row>
     <row r="44" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>7</v>
@@ -11673,7 +11679,7 @@
     </row>
     <row r="45" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>6</v>
@@ -11964,7 +11970,7 @@
     </row>
     <row r="46" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>5</v>
@@ -12381,7 +12387,7 @@
     </row>
     <row r="47" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>4</v>
@@ -12818,7 +12824,7 @@
     </row>
     <row r="48" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>3</v>
@@ -13229,7 +13235,7 @@
     </row>
     <row r="49" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>2</v>
@@ -13490,7 +13496,7 @@
     </row>
     <row r="50" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>1</v>
@@ -13937,7 +13943,7 @@
     </row>
     <row r="51" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
v4.17.0: AI Forecast v3.0 - New English prompt with Legacy Factor and All-Time Records
</commit_message>
<xml_diff>
--- a/Poker results.xlsx
+++ b/Poker results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liormol\projects\Poker Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B20AF2D-76C8-43EC-8C90-89C2B734A0B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D895A0D-B54A-4A32-8DD6-413A7B5D789F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{531639C6-E4BF-45C3-88E8-5B5EA68868B7}"/>
   </bookViews>
@@ -1633,11 +1633,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70A305C-45BC-4413-B0CD-355998277BD6}">
   <dimension ref="A11:HK51"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="11" spans="1:219" x14ac:dyDescent="0.25">
       <c r="A11" t="s">

</xml_diff>